<commit_message>
83: Modify the parameters data type of SRaw temperature compensation, from fixed integer to float type.  Named V0.37. (Date20250711)
</commit_message>
<xml_diff>
--- a/Objects/PGS7-0-36_202500708-BurnFile/PGS7_FW_ChangeNote.xlsx
+++ b/Objects/PGS7-0-36_202500708-BurnFile/PGS7_FW_ChangeNote.xlsx
@@ -973,7 +973,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -984,9 +984,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1340,7 +1337,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1867,7 +1864,7 @@
       <c r="B37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="1" t="s">

</xml_diff>